<commit_message>
inc i dec brightness
</commit_message>
<xml_diff>
--- a/STM32F7-MISS-TouchGFX_WRK/Application/Gui/assets/texts/texts.xlsx
+++ b/STM32F7-MISS-TouchGFX_WRK/Application/Gui/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="55">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -168,6 +168,18 @@
   </si>
   <si>
     <t xml:space="preserve">ver. 0.0.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New </t>
+  </si>
+  <si>
+    <t xml:space="preserve">+</t>
   </si>
 </sst>
 </file>
@@ -1607,6 +1619,7 @@
         <v>50</v>
       </c>
     </row>
+    <row r="6"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
informacja o jasności ekranu na LCD - do dopracowania
</commit_message>
<xml_diff>
--- a/STM32F7-MISS-TouchGFX_WRK/Application/Gui/assets/texts/texts.xlsx
+++ b/STM32F7-MISS-TouchGFX_WRK/Application/Gui/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="62">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -180,6 +180,27 @@
   </si>
   <si>
     <t xml:space="preserve">+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XX %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XX %&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt; %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0123456789-</t>
   </si>
 </sst>
 </file>
@@ -1405,7 +1426,9 @@
       <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="G4"/>
+      <c r="G4" t="s">
+        <v>61</v>
+      </c>
       <c r="H4"/>
       <c r="I4"/>
       <c r="K4" s="4" t="s">
@@ -1619,7 +1642,41 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6"/>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
work mode - nowy ekran
</commit_message>
<xml_diff>
--- a/STM32F7-MISS-TouchGFX_WRK/Application/Gui/assets/texts/texts.xlsx
+++ b/STM32F7-MISS-TouchGFX_WRK/Application/Gui/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="69">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -201,6 +201,27 @@
   </si>
   <si>
     <t xml:space="preserve">0123456789-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Device sett</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Device settings:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Work mode:</t>
   </si>
 </sst>
 </file>
@@ -1644,7 +1665,7 @@
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
         <v>37</v>
@@ -1661,7 +1682,7 @@
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C7" t="s">
         <v>37</v>
@@ -1676,7 +1697,40 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8"/>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
start i stop na panelu work mode i uruchomione czujnik oraz silnik
</commit_message>
<xml_diff>
--- a/STM32F7-MISS-TouchGFX_WRK/Application/Gui/assets/texts/texts.xlsx
+++ b/STM32F7-MISS-TouchGFX_WRK/Application/Gui/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3739" uniqueCount="177">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -222,6 +222,418 @@
   </si>
   <si>
     <t xml:space="preserve">Work mode:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual pressure </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow[l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow[l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0123456789-%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0123456789-% </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual 
+flow [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0123456789-%,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0123456789-%,.</t>
   </si>
 </sst>
 </file>
@@ -1448,7 +1860,7 @@
         <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>61</v>
+        <v>106</v>
       </c>
       <c r="H4"/>
       <c r="I4"/>
@@ -1469,6 +1881,26 @@
       </c>
     </row>
     <row r="5" spans="2:15">
+      <c r="B5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5">
+        <v>26</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>176</v>
+      </c>
+      <c r="H5"/>
+      <c r="I5"/>
       <c r="K5" s="7" t="s">
         <v>1</v>
       </c>
@@ -1731,6 +2163,159 @@
         <v>68</v>
       </c>
     </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" t="s">
+        <v>125</v>
+      </c>
+      <c r="D13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>149</v>
+      </c>
+      <c r="C14" t="s">
+        <v>125</v>
+      </c>
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s">
+        <v>162</v>
+      </c>
+      <c r="C15" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s">
+        <v>163</v>
+      </c>
+      <c r="C16" t="s">
+        <v>125</v>
+      </c>
+      <c r="D16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="s">
+        <v>164</v>
+      </c>
+      <c r="C17" t="s">
+        <v>125</v>
+      </c>
+      <c r="D17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="s">
+        <v>165</v>
+      </c>
+      <c r="C18" t="s">
+        <v>125</v>
+      </c>
+      <c r="D18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
poprawne wizualizowanie wildcards (bez automatycznego dopasowania do tekstu) + preset values
</commit_message>
<xml_diff>
--- a/STM32F7-MISS-TouchGFX_WRK/Application/Gui/assets/texts/texts.xlsx
+++ b/STM32F7-MISS-TouchGFX_WRK/Application/Gui/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3739" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26468" uniqueCount="325">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -634,6 +634,567 @@
   </si>
   <si>
     <t xml:space="preserve">0123456789-%,.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brightness:
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brightness:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&lt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preset
+pressure [mmHg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre
+flow [l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preset
+flow [l/min.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pres
+flow [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preset
+flow [rpm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Langu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Language:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
   </si>
 </sst>
 </file>
@@ -2100,7 +2661,7 @@
         <v>57</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>125</v>
       </c>
       <c r="D6" t="s">
         <v>52</v>
@@ -2109,7 +2670,7 @@
         <v>41</v>
       </c>
       <c r="F6" t="s">
-        <v>59</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7">
@@ -2117,7 +2678,7 @@
         <v>62</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>125</v>
       </c>
       <c r="D7" t="s">
         <v>52</v>
@@ -2245,7 +2806,7 @@
         <v>41</v>
       </c>
       <c r="F14" t="s">
-        <v>60</v>
+        <v>324</v>
       </c>
     </row>
     <row r="15">
@@ -2279,7 +2840,7 @@
         <v>41</v>
       </c>
       <c r="F16" t="s">
-        <v>60</v>
+        <v>250</v>
       </c>
     </row>
     <row r="17">
@@ -2316,6 +2877,211 @@
         <v>60</v>
       </c>
     </row>
+    <row r="19">
+      <c r="B19" t="s">
+        <v>178</v>
+      </c>
+      <c r="C19" t="s">
+        <v>125</v>
+      </c>
+      <c r="D19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="s">
+        <v>182</v>
+      </c>
+      <c r="C20" t="s">
+        <v>125</v>
+      </c>
+      <c r="D20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="s">
+        <v>185</v>
+      </c>
+      <c r="C21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="s">
+        <v>225</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="s">
+        <v>228</v>
+      </c>
+      <c r="C23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="s">
+        <v>231</v>
+      </c>
+      <c r="C24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="s">
+        <v>234</v>
+      </c>
+      <c r="C25" t="s">
+        <v>125</v>
+      </c>
+      <c r="D25" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C26" t="s">
+        <v>125</v>
+      </c>
+      <c r="D26" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="s">
+        <v>236</v>
+      </c>
+      <c r="C27" t="s">
+        <v>125</v>
+      </c>
+      <c r="D27" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" t="s">
+        <v>41</v>
+      </c>
+      <c r="F27" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="s">
+        <v>237</v>
+      </c>
+      <c r="C28" t="s">
+        <v>125</v>
+      </c>
+      <c r="D28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="s">
+        <v>238</v>
+      </c>
+      <c r="C29" t="s">
+        <v>125</v>
+      </c>
+      <c r="D29" t="s">
+        <v>52</v>
+      </c>
+      <c r="E29" t="s">
+        <v>41</v>
+      </c>
+      <c r="F29" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="s">
+        <v>239</v>
+      </c>
+      <c r="C30" t="s">
+        <v>125</v>
+      </c>
+      <c r="D30" t="s">
+        <v>40</v>
+      </c>
+      <c r="E30" t="s">
+        <v>41</v>
+      </c>
+      <c r="F30" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="31"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
mcu load na każdym ekranie i problem ze wspólnym interfejsem
</commit_message>
<xml_diff>
--- a/STM32F7-MISS-TouchGFX_WRK/Application/Gui/assets/texts/texts.xlsx
+++ b/STM32F7-MISS-TouchGFX_WRK/Application/Gui/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26468" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29738" uniqueCount="334">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1195,6 +1195,34 @@
   <si>
     <t xml:space="preserve">0
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCU Load: &lt;value&gt;%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T_DEMO_VIEW_MCU_LOAD_VALUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEMO_VIEW_MCU_LOAD_VALUE</t>
   </si>
 </sst>
 </file>
@@ -2421,7 +2449,7 @@
         <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>106</v>
+        <v>176</v>
       </c>
       <c r="H4"/>
       <c r="I4"/>
@@ -2794,75 +2822,75 @@
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="C14" t="s">
         <v>125</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="E14" t="s">
         <v>41</v>
       </c>
       <c r="F14" t="s">
-        <v>324</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C15" t="s">
         <v>125</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E15" t="s">
         <v>41</v>
       </c>
       <c r="F15" t="s">
-        <v>148</v>
+        <v>250</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C16" t="s">
         <v>125</v>
       </c>
       <c r="D16" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="E16" t="s">
         <v>41</v>
       </c>
       <c r="F16" t="s">
-        <v>250</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C17" t="s">
         <v>125</v>
       </c>
       <c r="D17" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E17" t="s">
         <v>41</v>
       </c>
       <c r="F17" t="s">
-        <v>148</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="C18" t="s">
         <v>125</v>
@@ -2874,12 +2902,12 @@
         <v>41</v>
       </c>
       <c r="F18" t="s">
-        <v>60</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="C19" t="s">
         <v>125</v>
@@ -2891,32 +2919,32 @@
         <v>41</v>
       </c>
       <c r="F19" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C20" t="s">
         <v>125</v>
       </c>
       <c r="D20" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="E20" t="s">
         <v>41</v>
       </c>
       <c r="F20" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="s">
-        <v>185</v>
+        <v>225</v>
       </c>
       <c r="C21" t="s">
-        <v>125</v>
+        <v>37</v>
       </c>
       <c r="D21" t="s">
         <v>52</v>
@@ -2925,12 +2953,12 @@
         <v>41</v>
       </c>
       <c r="F21" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C22" t="s">
         <v>37</v>
@@ -2942,12 +2970,12 @@
         <v>41</v>
       </c>
       <c r="F22" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="C23" t="s">
         <v>37</v>
@@ -2959,15 +2987,15 @@
         <v>41</v>
       </c>
       <c r="F23" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C24" t="s">
-        <v>37</v>
+        <v>125</v>
       </c>
       <c r="D24" t="s">
         <v>52</v>
@@ -2976,100 +3004,100 @@
         <v>41</v>
       </c>
       <c r="F24" t="s">
-        <v>233</v>
+        <v>148</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C25" t="s">
         <v>125</v>
       </c>
       <c r="D25" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E25" t="s">
         <v>41</v>
       </c>
       <c r="F25" t="s">
-        <v>148</v>
+        <v>246</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C26" t="s">
         <v>125</v>
       </c>
       <c r="D26" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="E26" t="s">
         <v>41</v>
       </c>
       <c r="F26" t="s">
-        <v>324</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C27" t="s">
         <v>125</v>
       </c>
       <c r="D27" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E27" t="s">
         <v>41</v>
       </c>
       <c r="F27" t="s">
-        <v>148</v>
+        <v>250</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C28" t="s">
         <v>125</v>
       </c>
       <c r="D28" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="E28" t="s">
         <v>41</v>
       </c>
       <c r="F28" t="s">
-        <v>250</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C29" t="s">
         <v>125</v>
       </c>
       <c r="D29" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E29" t="s">
         <v>41</v>
       </c>
       <c r="F29" t="s">
-        <v>148</v>
+        <v>246</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C30" t="s">
-        <v>125</v>
+        <v>37</v>
       </c>
       <c r="D30" t="s">
         <v>40</v>
@@ -3078,10 +3106,61 @@
         <v>41</v>
       </c>
       <c r="F30" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="31"/>
+        <v>325</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="s">
+        <v>326</v>
+      </c>
+      <c r="C31" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" t="s">
+        <v>41</v>
+      </c>
+      <c r="F31" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="s">
+        <v>331</v>
+      </c>
+      <c r="C32" t="s">
+        <v>125</v>
+      </c>
+      <c r="D32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32" t="s">
+        <v>41</v>
+      </c>
+      <c r="F32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="s">
+        <v>333</v>
+      </c>
+      <c r="C33" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E33" t="s">
+        <v>41</v>
+      </c>
+      <c r="F33" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="34"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
przechowywanie w model ustawień brightness i mcuload
</commit_message>
<xml_diff>
--- a/STM32F7-MISS-TouchGFX_WRK/Application/Gui/assets/texts/texts.xlsx
+++ b/STM32F7-MISS-TouchGFX_WRK/Application/Gui/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29738" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32029" uniqueCount="345">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1223,6 +1223,39 @@
   </si>
   <si>
     <t xml:space="preserve">DEMO_VIEW_MCU_LOAD_VALUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCU Load: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&gt; %</t>
   </si>
 </sst>
 </file>
@@ -3100,21 +3133,21 @@
         <v>37</v>
       </c>
       <c r="D30" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="E30" t="s">
         <v>41</v>
       </c>
       <c r="F30" t="s">
-        <v>325</v>
+        <v>191</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="C31" t="s">
-        <v>37</v>
+        <v>125</v>
       </c>
       <c r="D31" t="s">
         <v>40</v>
@@ -3123,15 +3156,15 @@
         <v>41</v>
       </c>
       <c r="F31" t="s">
-        <v>325</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C32" t="s">
-        <v>125</v>
+        <v>37</v>
       </c>
       <c r="D32" t="s">
         <v>40</v>
@@ -3140,12 +3173,12 @@
         <v>41</v>
       </c>
       <c r="F32" t="s">
-        <v>60</v>
+        <v>325</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C33" t="s">
         <v>37</v>
@@ -3157,10 +3190,112 @@
         <v>41</v>
       </c>
       <c r="F33" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="34"/>
+        <v>336</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="s">
+        <v>337</v>
+      </c>
+      <c r="C34" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" t="s">
+        <v>52</v>
+      </c>
+      <c r="E34" t="s">
+        <v>41</v>
+      </c>
+      <c r="F34" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="s">
+        <v>338</v>
+      </c>
+      <c r="C35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" t="s">
+        <v>40</v>
+      </c>
+      <c r="E35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F35" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="s">
+        <v>339</v>
+      </c>
+      <c r="C36" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" t="s">
+        <v>52</v>
+      </c>
+      <c r="E36" t="s">
+        <v>41</v>
+      </c>
+      <c r="F36" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="s">
+        <v>340</v>
+      </c>
+      <c r="C37" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" t="s">
+        <v>40</v>
+      </c>
+      <c r="E37" t="s">
+        <v>41</v>
+      </c>
+      <c r="F37" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="s">
+        <v>341</v>
+      </c>
+      <c r="C38" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38" t="s">
+        <v>52</v>
+      </c>
+      <c r="E38" t="s">
+        <v>41</v>
+      </c>
+      <c r="F38" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="s">
+        <v>342</v>
+      </c>
+      <c r="C39" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" t="s">
+        <v>40</v>
+      </c>
+      <c r="E39" t="s">
+        <v>41</v>
+      </c>
+      <c r="F39" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="40"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
porządek z nazwach kolejnych ekranów + możliwość zmiany z poziomu MODEL
</commit_message>
<xml_diff>
--- a/STM32F7-MISS-TouchGFX_WRK/Application/Gui/assets/texts/texts.xlsx
+++ b/STM32F7-MISS-TouchGFX_WRK/Application/Gui/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32029" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32969" uniqueCount="347">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1256,6 +1256,12 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;&gt; %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Autotest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Autotest:</t>
   </si>
 </sst>
 </file>
@@ -3295,7 +3301,23 @@
         <v>336</v>
       </c>
     </row>
-    <row r="40"/>
+    <row r="40">
+      <c r="B40" t="s">
+        <v>343</v>
+      </c>
+      <c r="C40" t="s">
+        <v>37</v>
+      </c>
+      <c r="D40" t="s">
+        <v>40</v>
+      </c>
+      <c r="E40" t="s">
+        <v>41</v>
+      </c>
+      <c r="F40" t="s">
+        <v>346</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
tryb LEVEL i dalsze prace porządkowe
</commit_message>
<xml_diff>
--- a/STM32F7-MISS-TouchGFX_WRK/Application/Gui/assets/texts/texts.xlsx
+++ b/STM32F7-MISS-TouchGFX_WRK/Application/Gui/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32969" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36210" uniqueCount="359">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1262,6 +1262,42 @@
   </si>
   <si>
     <t xml:space="preserve">Autotest:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnosti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnostic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnostics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnostics:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level:</t>
   </si>
 </sst>
 </file>
@@ -3315,9 +3351,61 @@
         <v>41</v>
       </c>
       <c r="F40" t="s">
-        <v>346</v>
-      </c>
-    </row>
+        <v>354</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" t="s">
+        <v>347</v>
+      </c>
+      <c r="C41" t="s">
+        <v>37</v>
+      </c>
+      <c r="D41" t="s">
+        <v>52</v>
+      </c>
+      <c r="E41" t="s">
+        <v>41</v>
+      </c>
+      <c r="F41" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" t="s">
+        <v>348</v>
+      </c>
+      <c r="C42" t="s">
+        <v>37</v>
+      </c>
+      <c r="D42" t="s">
+        <v>40</v>
+      </c>
+      <c r="E42" t="s">
+        <v>41</v>
+      </c>
+      <c r="F42" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" t="s">
+        <v>355</v>
+      </c>
+      <c r="C43" t="s">
+        <v>37</v>
+      </c>
+      <c r="D43" t="s">
+        <v>40</v>
+      </c>
+      <c r="E43" t="s">
+        <v>41</v>
+      </c>
+      <c r="F43" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="44"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
usunięte zbędne ekrany z prezentacji dla RK
</commit_message>
<xml_diff>
--- a/STM32F7-MISS-TouchGFX_WRK/Application/Gui/assets/texts/texts.xlsx
+++ b/STM32F7-MISS-TouchGFX_WRK/Application/Gui/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220726" uniqueCount="1910">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221557" uniqueCount="1910">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -9431,10 +9431,10 @@
     </row>
     <row r="38">
       <c r="B38" t="s">
-        <v>341</v>
+        <v>1201</v>
       </c>
       <c r="C38" t="s">
-        <v>37</v>
+        <v>125</v>
       </c>
       <c r="D38" t="s">
         <v>52</v>
@@ -9443,315 +9443,75 @@
         <v>41</v>
       </c>
       <c r="F38" t="s">
-        <v>191</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="s">
-        <v>342</v>
+        <v>1332</v>
       </c>
       <c r="C39" t="s">
-        <v>37</v>
+        <v>125</v>
       </c>
       <c r="D39" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="E39" t="s">
         <v>41</v>
       </c>
       <c r="F39" t="s">
-        <v>336</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="s">
-        <v>343</v>
+        <v>1427</v>
       </c>
       <c r="C40" t="s">
         <v>37</v>
       </c>
       <c r="D40" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="E40" t="s">
         <v>41</v>
       </c>
       <c r="F40" t="s">
-        <v>354</v>
+        <v>565</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="s">
-        <v>347</v>
+        <v>1582</v>
       </c>
       <c r="C41" t="s">
-        <v>37</v>
+        <v>125</v>
       </c>
       <c r="D41" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E41" t="s">
         <v>41</v>
       </c>
       <c r="F41" t="s">
-        <v>191</v>
+        <v>1813</v>
       </c>
     </row>
-    <row r="42">
-      <c r="B42" t="s">
-        <v>348</v>
-      </c>
-      <c r="C42" t="s">
-        <v>37</v>
-      </c>
-      <c r="D42" t="s">
-        <v>40</v>
-      </c>
-      <c r="E42" t="s">
-        <v>41</v>
-      </c>
-      <c r="F42" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="B43" t="s">
-        <v>355</v>
-      </c>
-      <c r="C43" t="s">
-        <v>37</v>
-      </c>
-      <c r="D43" t="s">
-        <v>40</v>
-      </c>
-      <c r="E43" t="s">
-        <v>41</v>
-      </c>
-      <c r="F43" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="B44" t="s">
-        <v>356</v>
-      </c>
-      <c r="C44" t="s">
-        <v>37</v>
-      </c>
-      <c r="D44" t="s">
-        <v>52</v>
-      </c>
-      <c r="E44" t="s">
-        <v>41</v>
-      </c>
-      <c r="F44" t="s">
-        <v>1907</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="B45" t="s">
-        <v>411</v>
-      </c>
-      <c r="C45" t="s">
-        <v>125</v>
-      </c>
-      <c r="D45" t="s">
-        <v>40</v>
-      </c>
-      <c r="E45" t="s">
-        <v>41</v>
-      </c>
-      <c r="F45" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="B46" t="s">
-        <v>561</v>
-      </c>
-      <c r="C46" t="s">
-        <v>37</v>
-      </c>
-      <c r="D46" t="s">
-        <v>52</v>
-      </c>
-      <c r="E46" t="s">
-        <v>41</v>
-      </c>
-      <c r="F46" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="B47" t="s">
-        <v>571</v>
-      </c>
-      <c r="C47" t="s">
-        <v>37</v>
-      </c>
-      <c r="D47" t="s">
-        <v>52</v>
-      </c>
-      <c r="E47" t="s">
-        <v>41</v>
-      </c>
-      <c r="F47" t="s">
-        <v>1908</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="B48" t="s">
-        <v>595</v>
-      </c>
-      <c r="C48" t="s">
-        <v>37</v>
-      </c>
-      <c r="D48" t="s">
-        <v>52</v>
-      </c>
-      <c r="E48" t="s">
-        <v>41</v>
-      </c>
-      <c r="F48" t="s">
-        <v>1909</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="B49" t="s">
-        <v>906</v>
-      </c>
-      <c r="C49" t="s">
-        <v>37</v>
-      </c>
-      <c r="D49" t="s">
-        <v>52</v>
-      </c>
-      <c r="E49" t="s">
-        <v>41</v>
-      </c>
-      <c r="F49" t="s">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="B50" t="s">
-        <v>938</v>
-      </c>
-      <c r="C50" t="s">
-        <v>125</v>
-      </c>
-      <c r="D50" t="s">
-        <v>177</v>
-      </c>
-      <c r="E50" t="s">
-        <v>41</v>
-      </c>
-      <c r="F50" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="B51" t="s">
-        <v>958</v>
-      </c>
-      <c r="C51" t="s">
-        <v>125</v>
-      </c>
-      <c r="D51" t="s">
-        <v>40</v>
-      </c>
-      <c r="E51" t="s">
-        <v>41</v>
-      </c>
-      <c r="F51" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="B52" t="s">
-        <v>976</v>
-      </c>
-      <c r="C52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D52" t="s">
-        <v>52</v>
-      </c>
-      <c r="E52" t="s">
-        <v>41</v>
-      </c>
-      <c r="F52" t="s">
-        <v>987</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="B53" t="s">
-        <v>1201</v>
-      </c>
-      <c r="C53" t="s">
-        <v>125</v>
-      </c>
-      <c r="D53" t="s">
-        <v>52</v>
-      </c>
-      <c r="E53" t="s">
-        <v>41</v>
-      </c>
-      <c r="F53" t="s">
-        <v>1208</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="B54" t="s">
-        <v>1332</v>
-      </c>
-      <c r="C54" t="s">
-        <v>125</v>
-      </c>
-      <c r="D54" t="s">
-        <v>52</v>
-      </c>
-      <c r="E54" t="s">
-        <v>41</v>
-      </c>
-      <c r="F54" t="s">
-        <v>1348</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="B55" t="s">
-        <v>1427</v>
-      </c>
-      <c r="C55" t="s">
-        <v>37</v>
-      </c>
-      <c r="D55" t="s">
-        <v>52</v>
-      </c>
-      <c r="E55" t="s">
-        <v>41</v>
-      </c>
-      <c r="F55" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="B56" t="s">
-        <v>1582</v>
-      </c>
-      <c r="C56" t="s">
-        <v>125</v>
-      </c>
-      <c r="D56" t="s">
-        <v>40</v>
-      </c>
-      <c r="E56" t="s">
-        <v>41</v>
-      </c>
-      <c r="F56" t="s">
-        <v>1813</v>
-      </c>
-    </row>
+    <row r="42"/>
+    <row r="43"/>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46"/>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50"/>
+    <row r="51"/>
+    <row r="52"/>
+    <row r="53"/>
+    <row r="54"/>
+    <row r="55"/>
+    <row r="56"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
statystyka błędów Carmen + nowe struktury przesyłane do GUI - zbyt duże MCU LOAD
</commit_message>
<xml_diff>
--- a/STM32F7-MISS-TouchGFX_WRK/Application/Gui/assets/texts/texts.xlsx
+++ b/STM32F7-MISS-TouchGFX_WRK/Application/Gui/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221557" uniqueCount="1910">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225996" uniqueCount="1929">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -7424,6 +7424,63 @@
   <si>
     <t xml:space="preserve">organ is placed
 below the device</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tempera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature [C]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valid / </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valid / E_CRC:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature [C]:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature [C]:sCarmenData_t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature [C]:&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;/&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1000000</t>
   </si>
 </sst>
 </file>
@@ -9497,13 +9554,125 @@
         <v>1813</v>
       </c>
     </row>
-    <row r="42"/>
-    <row r="43"/>
-    <row r="44"/>
-    <row r="45"/>
-    <row r="46"/>
-    <row r="47"/>
-    <row r="48"/>
+    <row r="42">
+      <c r="B42" t="s">
+        <v>1910</v>
+      </c>
+      <c r="C42" t="s">
+        <v>37</v>
+      </c>
+      <c r="D42" t="s">
+        <v>52</v>
+      </c>
+      <c r="E42" t="s">
+        <v>41</v>
+      </c>
+      <c r="F42" t="s">
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" t="s">
+        <v>1913</v>
+      </c>
+      <c r="C43" t="s">
+        <v>37</v>
+      </c>
+      <c r="D43" t="s">
+        <v>52</v>
+      </c>
+      <c r="E43" t="s">
+        <v>41</v>
+      </c>
+      <c r="F43" t="s">
+        <v>1915</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="B44" t="s">
+        <v>1918</v>
+      </c>
+      <c r="C44" t="s">
+        <v>37</v>
+      </c>
+      <c r="D44" t="s">
+        <v>40</v>
+      </c>
+      <c r="E44" t="s">
+        <v>41</v>
+      </c>
+      <c r="F44" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" t="s">
+        <v>1920</v>
+      </c>
+      <c r="C45" t="s">
+        <v>37</v>
+      </c>
+      <c r="D45" t="s">
+        <v>40</v>
+      </c>
+      <c r="E45" t="s">
+        <v>41</v>
+      </c>
+      <c r="F45" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" t="s">
+        <v>1921</v>
+      </c>
+      <c r="C46" t="s">
+        <v>37</v>
+      </c>
+      <c r="D46" t="s">
+        <v>52</v>
+      </c>
+      <c r="E46" t="s">
+        <v>41</v>
+      </c>
+      <c r="F46" t="s">
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" t="s">
+        <v>1924</v>
+      </c>
+      <c r="C47" t="s">
+        <v>37</v>
+      </c>
+      <c r="D47" t="s">
+        <v>40</v>
+      </c>
+      <c r="E47" t="s">
+        <v>41</v>
+      </c>
+      <c r="F47" t="s">
+        <v>1926</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" t="s">
+        <v>1927</v>
+      </c>
+      <c r="C48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D48" t="s">
+        <v>40</v>
+      </c>
+      <c r="E48" t="s">
+        <v>41</v>
+      </c>
+      <c r="F48" t="s">
+        <v>1928</v>
+      </c>
+    </row>
     <row r="49"/>
     <row r="50"/>
     <row r="51"/>

</xml_diff>

<commit_message>
odczyt diagnostyki silnika na GUI
</commit_message>
<xml_diff>
--- a/STM32F7-MISS-TouchGFX_WRK/Application/Gui/assets/texts/texts.xlsx
+++ b/STM32F7-MISS-TouchGFX_WRK/Application/Gui/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225996" uniqueCount="1929">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227200" uniqueCount="1935">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -7481,6 +7481,24 @@
   </si>
   <si>
     <t xml:space="preserve">1000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motor Diagn:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65535</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId72</t>
   </si>
 </sst>
 </file>
@@ -9673,10 +9691,74 @@
         <v>1928</v>
       </c>
     </row>
-    <row r="49"/>
-    <row r="50"/>
-    <row r="51"/>
-    <row r="52"/>
+    <row r="49">
+      <c r="B49" t="s">
+        <v>1929</v>
+      </c>
+      <c r="C49" t="s">
+        <v>37</v>
+      </c>
+      <c r="D49" t="s">
+        <v>52</v>
+      </c>
+      <c r="E49" t="s">
+        <v>41</v>
+      </c>
+      <c r="F49" t="s">
+        <v>1930</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" t="s">
+        <v>1931</v>
+      </c>
+      <c r="C50" t="s">
+        <v>37</v>
+      </c>
+      <c r="D50" t="s">
+        <v>52</v>
+      </c>
+      <c r="E50" t="s">
+        <v>41</v>
+      </c>
+      <c r="F50" t="s">
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" t="s">
+        <v>1932</v>
+      </c>
+      <c r="C51" t="s">
+        <v>37</v>
+      </c>
+      <c r="D51" t="s">
+        <v>40</v>
+      </c>
+      <c r="E51" t="s">
+        <v>41</v>
+      </c>
+      <c r="F51" t="s">
+        <v>1933</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="B52" t="s">
+        <v>1934</v>
+      </c>
+      <c r="C52" t="s">
+        <v>37</v>
+      </c>
+      <c r="D52" t="s">
+        <v>40</v>
+      </c>
+      <c r="E52" t="s">
+        <v>41</v>
+      </c>
+      <c r="F52" t="s">
+        <v>1933</v>
+      </c>
+    </row>
     <row r="53"/>
     <row r="54"/>
     <row r="55"/>

</xml_diff>